<commit_message>
now i can update tag and reply
</commit_message>
<xml_diff>
--- a/pandora_scraper/pandora_export.xlsx
+++ b/pandora_scraper/pandora_export.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="101">
   <si>
     <t>Message_Time</t>
   </si>
@@ -31,87 +31,6 @@
   </si>
   <si>
     <t>URL</t>
-  </si>
-  <si>
-    <t>Thursday, February 06, 2020 01:33:13 AM</t>
-  </si>
-  <si>
-    <t>Kaman Ho</t>
-  </si>
-  <si>
-    <t>Pandora …不了🤗</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/153753694819713/posts/1249085878619817/?comment_id=1252958851565853</t>
-  </si>
-  <si>
-    <t>Thursday, February 06, 2020 03:09:49 AM</t>
-  </si>
-  <si>
-    <t>Grace Wong</t>
-  </si>
-  <si>
-    <t>只是買設計 價值何在 只有喜歡而喜歡而已</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/153753694819713/posts/1249085878619817/?comment_id=1253009371560801</t>
-  </si>
-  <si>
-    <t>Thursday, February 06, 2020 04:03:21 AM</t>
-  </si>
-  <si>
-    <t>Hong Jai</t>
-  </si>
-  <si>
-    <t>成本幾蚊炒到幾百蚊粒，仲離譜過啲口罩</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/153753694819713/posts/1251795725015499/?comment_id=1253033928225012</t>
-  </si>
-  <si>
-    <t>Thursday, February 06, 2020 10:13:55 AM</t>
-  </si>
-  <si>
-    <t>Lok Daisy</t>
-  </si>
-  <si>
-    <t>拎條鍊去洗，會屈你條鍊用洗銀水浸過，然後同你講洗唔到原來既色架！仲買？</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/153753694819713/posts/1253098498218555/?comment_id=1253209688207436</t>
-  </si>
-  <si>
-    <t>Thursday, February 06, 2020 10:31:26 AM</t>
-  </si>
-  <si>
-    <t>Minmin Cheung</t>
-  </si>
-  <si>
-    <t>仲有人買既咩</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/PandoraHongKong/photos/a.156393951222354/1249078298620575/?type=3&amp;comment_id=1253217394873332</t>
-  </si>
-  <si>
-    <t>Thursday, February 06, 2020 10:44:50 AM</t>
-  </si>
-  <si>
-    <t>Pandora 不如你話我知，我咁樣俾人屈，你地可以點協助我？</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/153753694819713/posts/1249085878619817/?comment_id=1251110855083986&amp;reply_comment_id=1253223401539398</t>
-  </si>
-  <si>
-    <t>Thursday, February 06, 2020 10:49:35 AM</t>
-  </si>
-  <si>
-    <t>安李</t>
-  </si>
-  <si>
-    <t>Hm</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/PandoraHongKong/photos/a.156393951222354/955925041269237/?type=3&amp;comment_id=1253225584872513</t>
   </si>
   <si>
     <t>Thursday, February 06, 2020 02:28:07 PM</t>
@@ -140,16 +59,88 @@
     <t>https://www.facebook.com/153753694819713/posts/1251808008347604/?comment_id=1253322551529483</t>
   </si>
   <si>
-    <t>Sunday, December 29, 2019 07:17:43 PM</t>
+    <t>Thursday, February 06, 2020 04:42:38 PM</t>
   </si>
   <si>
-    <t>Bo Kei Fan</t>
+    <t>Lok Daisy</t>
+  </si>
+  <si>
+    <t>拎條鍊去洗，會屈你條鍊用洗銀水浸過，然後同你講洗唔到原來既色架！仲買？</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/153753694819713/posts/2240275839408885/?comment_id=2240277299408739</t>
+  </si>
+  <si>
+    <t>Thursday, February 06, 2020 06:58:27 PM</t>
+  </si>
+  <si>
+    <t>Beau Manuswee</t>
+  </si>
+  <si>
+    <t>Gift Kumpunthong อิอิ เพื่อคันๆๆๆ</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/153753694819713/posts/1249085878619817/?comment_id=1253444781517260</t>
+  </si>
+  <si>
+    <t>Thursday, February 06, 2020 09:43:47 PM</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/153753694819713/posts/2790696994324388/?comment_id=2790697870990967</t>
+  </si>
+  <si>
+    <t>Thursday, February 06, 2020 11:28:10 PM</t>
+  </si>
+  <si>
+    <t>May Yuen</t>
+  </si>
+  <si>
+    <t>請問米奇要幾錢</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/153753694819713/posts/1242183959310009/?comment_id=1253608004834271</t>
+  </si>
+  <si>
+    <t>Friday, February 07, 2020 08:31:24 AM</t>
+  </si>
+  <si>
+    <t>Mavis Law</t>
+  </si>
+  <si>
+    <t>Koey Wai Cherry Yeung</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/153753694819713/posts/1251251691736569/?comment_id=1253890828139322</t>
+  </si>
+  <si>
+    <t>Saturday, December 28, 2019 06:28:07 PM</t>
+  </si>
+  <si>
+    <t>Ha Tang</t>
   </si>
   <si>
     <t>Can I reserve this?</t>
   </si>
   <si>
     <t>Inbox</t>
+  </si>
+  <si>
+    <t>Sunday, December 29, 2019 12:54:31 AM</t>
+  </si>
+  <si>
+    <t>GY Yau</t>
+  </si>
+  <si>
+    <t>Sunday, December 29, 2019 11:53:06 AM</t>
+  </si>
+  <si>
+    <t>Edith Leung</t>
+  </si>
+  <si>
+    <t>Sunday, December 29, 2019 07:17:43 PM</t>
+  </si>
+  <si>
+    <t>Bo Kei Fan</t>
   </si>
   <si>
     <t>Sunday, December 29, 2019 10:35:28 PM</t>
@@ -174,27 +165,6 @@
   </si>
   <si>
     <t>我已經電郵了pap.cs@Pandora.net，但Katie沒有提供令人滿意的答覆，加上除此以外也沒有人回覆。她說我退回貨品後幾天可收回款項，但已經12天了，若然再沒有回覆，我會到警署和海關備案。</t>
-  </si>
-  <si>
-    <t>Thursday, February 06, 2020 01:49:02 AM</t>
-  </si>
-  <si>
-    <t>Emily Cheung</t>
-  </si>
-  <si>
-    <t>How many days does it take to deliver?</t>
-  </si>
-  <si>
-    <t>Thursday, February 06, 2020 01:49:25 AM</t>
-  </si>
-  <si>
-    <t>Sent wrongly</t>
-  </si>
-  <si>
-    <t>Thursday, February 06, 2020 07:13:39 AM</t>
-  </si>
-  <si>
-    <t>Wind Indah</t>
   </si>
   <si>
     <t>Thursday, February 06, 2020 02:33:51 PM</t>
@@ -1496,7 +1466,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
@@ -1579,69 +1549,41 @@
         <v>20</v>
       </c>
       <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
         <v>21</v>
-      </c>
-      <c r="C6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" t="s">
         <v>24</v>
       </c>
-      <c r="B7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>25</v>
-      </c>
-      <c r="D7" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
         <v>27</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>28</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>29</v>
-      </c>
-      <c r="D8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" t="s">
-        <v>31</v>
-      </c>
-      <c r="B9" t="s">
-        <v>32</v>
-      </c>
-      <c r="C9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" t="s">
-        <v>35</v>
-      </c>
-      <c r="B10" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10" t="s">
-        <v>37</v>
-      </c>
-      <c r="D10" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1679,114 +1621,114 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="C2" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="D2" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="C3" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="D3" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="C4" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="D4" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="B5" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="C5" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="D5" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="B6" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="C6" t="s">
-        <v>53</v>
+        <v>32</v>
       </c>
       <c r="D6" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="B7" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="C7" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="D7" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="B8" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="C8" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D8" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="B9" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="C9" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="D9" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1817,25 +1759,25 @@
   <sheetData>
     <row customFormat="1" r="1" s="16" spans="1:7">
       <c r="A1" s="16" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="D1" s="16" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="F1" s="16" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="16" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
     </row>
     <row customFormat="1" r="2" s="16" spans="1:7">
@@ -1955,7 +1897,7 @@
         <v/>
       </c>
       <c r="E6" s="16" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="F6" s="16">
         <f>Public!D6</f>
@@ -7944,25 +7886,25 @@
   <sheetData>
     <row customFormat="1" r="1" s="16" spans="1:7">
       <c r="A1" s="16" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="D1" s="16" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="F1" s="16" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="16" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
     </row>
     <row customFormat="1" r="2" s="16" spans="1:7">
@@ -14076,34 +14018,34 @@
   <sheetData>
     <row customFormat="1" customHeight="1" ht="28" r="1" s="1" spans="1:16384">
       <c r="A1" s="1" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="B1" s="21" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
     </row>
     <row customFormat="1" r="2" s="1" spans="1:16384">
@@ -14144,7 +14086,7 @@
         <v/>
       </c>
       <c r="J2" s="1" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
     </row>
     <row customFormat="1" r="3" s="1" spans="1:16384">
@@ -14337,7 +14279,7 @@
         <v/>
       </c>
       <c r="J7" s="1" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
     </row>
     <row customFormat="1" r="8" s="1" spans="1:16384">
@@ -14378,7 +14320,7 @@
         <v/>
       </c>
       <c r="J8" s="1" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
     </row>
     <row customFormat="1" r="9" s="1" spans="1:16384">
@@ -40323,34 +40265,34 @@
   <sheetData>
     <row customFormat="1" r="1" s="1" spans="1:8">
       <c r="A1" s="1" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="B1" s="21" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row customFormat="1" r="2" s="1" spans="1:8">
       <c r="B2" s="20" t="n"/>
       <c r="E2" s="1" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="G2" s="3" t="n"/>
       <c r="H2" s="4" t="n"/>
@@ -40365,22 +40307,22 @@
         <v>33</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="H4" s="4" t="n"/>
     </row>
@@ -40396,174 +40338,174 @@
     </row>
     <row customFormat="1" r="7" s="1" spans="1:8">
       <c r="B7" s="20" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="E7" s="1" t="n"/>
       <c r="F7" s="1" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="H7" s="4" t="n"/>
     </row>
     <row customFormat="1" r="8" s="1" spans="1:8">
       <c r="B8" s="20" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="E8" s="1" t="n"/>
       <c r="F8" s="1" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="H8" s="4" t="n"/>
     </row>
     <row customFormat="1" r="9" s="1" spans="1:8">
       <c r="B9" s="20" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="E9" s="1" t="n"/>
       <c r="F9" s="1" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="H9" s="4" t="n"/>
     </row>
     <row customFormat="1" r="10" s="1" spans="1:8">
       <c r="B10" s="20" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="E10" s="1" t="n"/>
       <c r="F10" s="1" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="H10" s="4" t="n"/>
     </row>
     <row customFormat="1" r="11" s="1" spans="1:8">
       <c r="B11" s="20" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="H11" s="4" t="n"/>
     </row>
     <row customFormat="1" r="12" s="1" spans="1:8">
       <c r="B12" s="20" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="E12" s="1" t="n"/>
       <c r="F12" s="1" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="H12" s="4" t="n"/>
     </row>
     <row customFormat="1" r="13" s="1" spans="1:8">
       <c r="B13" s="20" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E13" s="1" t="n"/>
       <c r="F13" s="1" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="H13" s="4" t="n"/>
     </row>
     <row customFormat="1" r="14" s="1" spans="1:8">
       <c r="B14" s="20" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E14" s="1" t="n"/>
       <c r="F14" s="1" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="H14" s="4" t="n"/>
     </row>
     <row customFormat="1" r="15" s="1" spans="1:8">
       <c r="B15" s="20" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="E15" s="1" t="n"/>
       <c r="F15" s="1" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="H15" s="4" t="n"/>
     </row>

</xml_diff>

<commit_message>
now i can reply to both inbox and comment yayyyy
</commit_message>
<xml_diff>
--- a/pandora_scraper/pandora_export.xlsx
+++ b/pandora_scraper/pandora_export.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="73">
   <si>
     <t>Message_Time</t>
   </si>
@@ -33,171 +33,155 @@
     <t>URL</t>
   </si>
   <si>
-    <t>Thursday, February 06, 2020 02:28:07 PM</t>
+    <t>Monday, February 10, 2020 08:20:11 PM</t>
   </si>
   <si>
-    <t>Helen Helen</t>
+    <t>陳初九</t>
   </si>
   <si>
-    <t>我都覺得呢個牌子唔應該再買，因脱色好緊要。</t>
+    <t>送口罩俾對方會唔會更體貼？</t>
   </si>
   <si>
-    <t>https://www.facebook.com/153753694819713/posts/1249085878619817/?comment_id=1253319778196427</t>
+    <t>https://www.facebook.com/PandoraHongKong/photos/a.156393951222354/1255043328024072/?type=3&amp;comment_id=1256554271206311</t>
   </si>
   <si>
-    <t>Thursday, February 06, 2020 02:35:47 PM</t>
+    <t>Monday, February 10, 2020 08:22:23 PM</t>
   </si>
   <si>
-    <t>Keith Hang</t>
+    <t>吳天豐</t>
   </si>
   <si>
-    <t>口罩漂白水酒精
-溝死女
-駛Q買你d珠仔💪🏻</t>
+    <t>圖中二人有否先洗手？</t>
   </si>
   <si>
-    <t>https://www.facebook.com/153753694819713/posts/1251808008347604/?comment_id=1253322551529483</t>
+    <t>https://www.facebook.com/PandoraHongKong/photos/a.156393951222354/1255043328024072/?type=3&amp;comment_id=1256555641206174</t>
   </si>
   <si>
-    <t>Thursday, February 06, 2020 04:42:38 PM</t>
+    <t>Monday, February 10, 2020 08:36:42 PM</t>
   </si>
   <si>
-    <t>Lok Daisy</t>
+    <t>Tszyeung Li</t>
   </si>
   <si>
-    <t>拎條鍊去洗，會屈你條鍊用洗銀水浸過，然後同你講洗唔到原來既色架！仲買？</t>
+    <t>港女鏈</t>
   </si>
   <si>
-    <t>https://www.facebook.com/153753694819713/posts/2240275839408885/?comment_id=2240277299408739</t>
+    <t>https://www.facebook.com/PandoraHongKong/photos/a.156393951222354/1255043328024072/?type=3&amp;comment_id=1256563117872093</t>
   </si>
   <si>
-    <t>Thursday, February 06, 2020 06:58:27 PM</t>
+    <t>Monday, February 10, 2020 10:53:00 PM</t>
   </si>
   <si>
-    <t>Beau Manuswee</t>
+    <t>Jason Wong</t>
   </si>
   <si>
-    <t>Gift Kumpunthong อิอิ เพื่อคันๆๆๆ</t>
+    <t>咁多首飾品牌，我最佩服Pandora，公園石春都賣到錢。。。。</t>
   </si>
   <si>
-    <t>https://www.facebook.com/153753694819713/posts/1249085878619817/?comment_id=1253444781517260</t>
+    <t>https://www.facebook.com/PandoraHongKong/photos/a.156393951222354/1255043328024072/?type=3&amp;comment_id=1256644537863951</t>
   </si>
   <si>
-    <t>Thursday, February 06, 2020 11:28:10 PM</t>
+    <t>Monday, February 10, 2020 03:42:11 PM</t>
   </si>
   <si>
-    <t>May Yuen</t>
+    <t>Leung Wan Ko</t>
   </si>
   <si>
-    <t>請問米奇要幾錢</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/153753694819713/posts/1242183959310009/?comment_id=1253608004834271</t>
-  </si>
-  <si>
-    <t>Friday, February 07, 2020 08:31:24 AM</t>
-  </si>
-  <si>
-    <t>Mavis Law</t>
-  </si>
-  <si>
-    <t>Koey Wai Cherry Yeung</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/153753694819713/posts/1251251691736569/?comment_id=1253890828139322</t>
-  </si>
-  <si>
-    <t>Friday, February 07, 2020 12:03:19 PM</t>
-  </si>
-  <si>
-    <t>Fanny Tam</t>
-  </si>
-  <si>
-    <t>買滿幾錢？</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/153753694819713/posts/1251251691736569/?comment_id=1253995441462194</t>
-  </si>
-  <si>
-    <t>Friday, February 07, 2020 01:49:29 PM</t>
-  </si>
-  <si>
-    <t>Keong Keong</t>
-  </si>
-  <si>
-    <t>就像愛情，找帥哥破處X膜，然後被拋棄，留下永久撕裂傷，開始放盪，在去做處X膜手術，然後找好騙工具人，一帥哥渣男多處X制，聽歌聽到腦殘，該感動不感動，亂享受感動，越漂亮曾墮胎機率越高👺👺👺👹👹👹</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/PandoraHongKong/photos/a.156393951222354/1251221261739612/?type=3&amp;comment_id=1254066051455133</t>
-  </si>
-  <si>
-    <t>Friday, February 07, 2020 02:23:06 PM</t>
-  </si>
-  <si>
-    <t>Cherry Yeung</t>
-  </si>
-  <si>
-    <t>Mavis Law 咁要集結去睇喎🤣</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/153753694819713/posts/1251251691736569/?comment_id=1253890828139322&amp;reply_comment_id=1254083041453434</t>
-  </si>
-  <si>
-    <t>Wednesday, January 08, 2020 12:08:11 PM</t>
-  </si>
-  <si>
-    <t>Anna Fung</t>
-  </si>
-  <si>
-    <t>我肯定你post嘅時候大部份早已冇貨！咁係咪要問問海關商品說明條例呢？</t>
+    <t>https://s3.amazonaws.com/spr-uploads-prod/815/FACEBOOK/82906/media/871187EE4A4126C860B609668FFB1D47</t>
   </si>
   <si>
     <t>Inbox</t>
   </si>
   <si>
-    <t>Wednesday, January 08, 2020 03:49:10 PM</t>
+    <t>Monday, February 10, 2020 03:42:34 PM</t>
   </si>
   <si>
-    <t>Bleu Loi</t>
+    <t>請問還有哩只款嗎？</t>
   </si>
   <si>
-    <t>我已經電郵了pap.cs@Pandora.net，但Katie沒有提供令人滿意的答覆，加上除此以外也沒有人回覆。她說我退回貨品後幾天可收回款項，但已經12天了，若然再沒有回覆，我會到警署和海關備案。</t>
+    <t>Monday, February 10, 2020 05:25:54 PM</t>
   </si>
   <si>
-    <t>Thursday, February 06, 2020 02:33:51 PM</t>
+    <t>Wan Pong Tang</t>
   </si>
   <si>
-    <t>Kathy Ching</t>
+    <t>昨日落了order，今日未見有mail confirm，可以幫我跟進嗎？
+order no. PNDHK00668968</t>
   </si>
   <si>
-    <t>i wanted to ask if there's stock of harry potter series in kings cross shop.  i have purchased on Tuesday already, thx</t>
+    <t>Monday, February 10, 2020 05:37:24 PM</t>
   </si>
   <si>
-    <t>Friday, February 07, 2020 01:16:07 PM</t>
+    <t>Dave Henz</t>
   </si>
   <si>
-    <t>Typ Wong</t>
+    <t>Hi</t>
   </si>
   <si>
-    <t>https://ezone.ulifestyle.com.hk/article/2557002
-【口罩開賣】理的口罩 HKTVmall 開賣！＄65 三十個！【附直購連結】 - ezone.hk - 網絡生活…
-l.facebook.com</t>
+    <t>Monday, February 10, 2020 05:37:38 PM</t>
   </si>
   <si>
-    <t>Friday, February 07, 2020 02:42:50 PM</t>
+    <t>I want to order this item</t>
   </si>
   <si>
-    <t>Lillian Li</t>
+    <t>Monday, February 10, 2020 05:37:43 PM</t>
   </si>
   <si>
-    <t>我門市買夠數，有9折，已經試過起門市用到9折，但網上又話我電話沒有登記，請跟進！
-Tel: 62906286</t>
+    <t>do you have</t>
   </si>
   <si>
-    <t>Friday, February 07, 2020 02:43:06 PM</t>
+    <t>Monday, February 10, 2020 05:37:48 PM</t>
   </si>
   <si>
-    <t>https://s3.amazonaws.com/spr-uploads-prod/815/FACEBOOK/82906/media/F288E0AB9EF90AFF734CCA123FC44B2A</t>
+    <t>https://s3.amazonaws.com/spr-uploads-prod/815/FACEBOOK/82906/media/F279C2ECD2CC380F0E54A0B4103F302C</t>
+  </si>
+  <si>
+    <t>Monday, February 10, 2020 06:28:45 PM</t>
+  </si>
+  <si>
+    <t>Tim Wong</t>
+  </si>
+  <si>
+    <t>請問現在落單13號或之前能收到嗎</t>
+  </si>
+  <si>
+    <t>Monday, February 10, 2020 06:56:08 PM</t>
+  </si>
+  <si>
+    <t>Asellus Wong</t>
+  </si>
+  <si>
+    <t>想問買滿$1380 送嘅頸鏈有幾長? 同埋個心心鏈嘴可唔可以拆落黎?</t>
+  </si>
+  <si>
+    <t>Monday, February 10, 2020 07:19:16 PM</t>
+  </si>
+  <si>
+    <t>順丰有資料了，thanks</t>
+  </si>
+  <si>
+    <t>Monday, February 10, 2020 11:29:52 PM</t>
+  </si>
+  <si>
+    <t>Noona Rt</t>
+  </si>
+  <si>
+    <t>你好，請問你地門巿有冇呢款耳環？</t>
+  </si>
+  <si>
+    <t>Monday, February 10, 2020 11:29:56 PM</t>
+  </si>
+  <si>
+    <t>https://s3.amazonaws.com/spr-uploads-prod/815/FACEBOOK/82906/media/166DD8C359D7B67ECCE9B0BE8F585988</t>
+  </si>
+  <si>
+    <t>Tuesday, February 11, 2020 10:52:57 AM</t>
+  </si>
+  <si>
+    <t>Mabel Lam</t>
+  </si>
+  <si>
+    <t>如果直接落門市有呢個款嗎？</t>
   </si>
   <si>
     <t>order</t>
@@ -242,80 +226,19 @@
     <t>Reply</t>
   </si>
   <si>
-    <t>Thursday, February 06, 2020 14:28:07</t>
+    <t>Monday, February 10, 2020 17:37:48</t>
   </si>
   <si>
-    <t>Hi Helen Helen，非常抱歉你有以上經歷。請你電郵至 pap.cs@Pandora.net 提供姓名、聯絡電話同詳情，我哋會作出跟進。多謝！</t>
-  </si>
-  <si>
-    <t>Complaints</t>
-  </si>
-  <si>
-    <t>Thursday, February 06, 2020 14:35:47</t>
-  </si>
-  <si>
-    <t>Other</t>
-  </si>
-  <si>
-    <t>Thursday, February 06, 2020 16:42:38</t>
-  </si>
-  <si>
-    <t>Thursday, February 06, 2020 18:58:27</t>
-  </si>
-  <si>
-    <t>Thursday, February 06, 2020 21:43:47</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/153753694819713/posts/2790696994324388/?comment_id=2790697870990967</t>
-  </si>
-  <si>
-    <t>Thursday, February 06, 2020 23:28:10</t>
-  </si>
-  <si>
-    <t>Hi May Yuen，請到 https://go.pandora.net/2SqrqAj 查閱價錢，多謝你嘅支持！</t>
+    <t>te</t>
   </si>
   <si>
     <t>General</t>
   </si>
   <si>
-    <t>Friday, February 07, 2020 08:31:24</t>
+    <t>Monday, February 10, 2020 23:29:52</t>
   </si>
   <si>
-    <t>Thursday, February 06, 2020 14:33:51</t>
-  </si>
-  <si>
-    <t>Hi Kathy Ching, thanks for supporting us! Love Pandora!</t>
-  </si>
-  <si>
-    <t>Friday, February 07, 2020 12:03:19</t>
-  </si>
-  <si>
-    <t>Hi Fanny Tam，而家喺網店同專門店消費淨值滿港幣$1,380，即可獲贈指定項鏈；
-淨值滿港幣$2,280，即可獲贈指定項鏈及耳環。優惠去到2020年2月15日 00:00，贈品數量有限，送完即止。多謝支持Pandora！</t>
-  </si>
-  <si>
-    <t>Friday, February 07, 2020 13:49:29</t>
-  </si>
-  <si>
-    <t>Hide this comment, mark as spam</t>
-  </si>
-  <si>
-    <t>Friday, February 07, 2020 14:23:06</t>
-  </si>
-  <si>
-    <t>Friday, February 07, 2020 13:16:07</t>
-  </si>
-  <si>
-    <t>https://ezone.ulifestyle.com.hk/article/2557002</t>
-  </si>
-  <si>
-    <t>Friday, February 07, 2020 14:42:50</t>
-  </si>
-  <si>
-    <t>Hi Lillian Li，非常抱歉你有以上經歷。請你電郵至 pap.cs@Pandora.net 提供姓名、聯絡電話同詳情，我哋會作出跟進。多謝你嘅支持！</t>
-  </si>
-  <si>
-    <t>Friday, February 07, 2020 14:43:06</t>
+    <t>ttt</t>
   </si>
 </sst>
 </file>
@@ -366,9 +289,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -382,9 +319,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -392,20 +328,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -420,7 +342,69 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -435,46 +419,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -483,28 +428,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -537,7 +460,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -549,37 +568,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -591,133 +628,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -789,17 +712,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -830,30 +742,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -871,9 +759,44 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -894,10 +817,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0">
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="7">
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="6">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0">
@@ -906,16 +829,16 @@
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0">
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0">
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0">
@@ -927,112 +850,112 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="10">
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="7">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0">
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0">
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="12">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="12">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0">
+    <xf numFmtId="0" fontId="6" fillId="35" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="6">
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="5">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="7">
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="6">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="9">
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="11">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="30" borderId="0">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0">
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="11">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0">
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0">
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="0">
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0">
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0">
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="0">
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="0">
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0">
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0">
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0">
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="28" borderId="0">
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="31" borderId="0">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="35" borderId="0">
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0">
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0">
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="34" borderId="0">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0">
+    <xf numFmtId="0" fontId="6" fillId="34" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1436,13 +1359,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="4" outlineLevelCol="3"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="16" t="s">
@@ -1512,76 +1435,6 @@
       </c>
       <c r="D5" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" t="s">
-        <v>32</v>
-      </c>
-      <c r="B9" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" t="s">
-        <v>34</v>
-      </c>
-      <c r="D9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" t="s">
-        <v>36</v>
-      </c>
-      <c r="B10" t="s">
-        <v>37</v>
-      </c>
-      <c r="C10" t="s">
-        <v>38</v>
-      </c>
-      <c r="D10" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1593,13 +1446,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J19" sqref="J19:J20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="6" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="3"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="16" t="s">
@@ -1617,86 +1470,184 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="D3" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>26</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
       <c r="C4" t="s">
-        <v>49</v>
+        <v>28</v>
       </c>
       <c r="D4" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>30</v>
       </c>
       <c r="C5" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="D5" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>53</v>
+        <v>32</v>
       </c>
       <c r="B6" t="s">
-        <v>54</v>
+        <v>30</v>
       </c>
       <c r="C6" t="s">
-        <v>55</v>
+        <v>33</v>
       </c>
       <c r="D6" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="B7" t="s">
-        <v>54</v>
+        <v>30</v>
       </c>
       <c r="C7" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
       <c r="D7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" t="s">
         <v>43</v>
+      </c>
+      <c r="D10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1711,7 +1662,7 @@
   <dimension ref="A1:G572"/>
   <sheetViews>
     <sheetView showZeros="0" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:G8"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14" outlineLevelCol="6"/>
@@ -1725,25 +1676,25 @@
   <sheetData>
     <row r="1" s="14" customFormat="1" spans="1:7">
       <c r="A1" s="14" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D1" s="14" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F1" s="14" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" s="14" customFormat="1" spans="1:7">
@@ -1752,19 +1703,19 @@
       </c>
       <c r="B2" s="6" t="str">
         <f>Public!A2</f>
-        <v>Thursday, February 06, 2020 02:28:07 PM</v>
+        <v>Monday, February 10, 2020 08:20:11 PM</v>
       </c>
       <c r="C2" s="14" t="str">
         <f>Public!B2</f>
-        <v>Helen Helen</v>
+        <v>陳初九</v>
       </c>
       <c r="D2" s="14" t="str">
         <f>Public!C2</f>
-        <v>我都覺得呢個牌子唔應該再買，因脱色好緊要。</v>
+        <v>送口罩俾對方會唔會更體貼？</v>
       </c>
       <c r="F2" s="14" t="str">
         <f>Public!D2</f>
-        <v>https://www.facebook.com/153753694819713/posts/1249085878619817/?comment_id=1253319778196427</v>
+        <v>https://www.facebook.com/PandoraHongKong/photos/a.156393951222354/1255043328024072/?type=3&amp;comment_id=1256554271206311</v>
       </c>
       <c r="G2" s="3" t="str">
         <f t="shared" ref="G2:G65" si="0">IF(E2="No response required","Other","")</f>
@@ -1777,21 +1728,19 @@
       </c>
       <c r="B3" s="6" t="str">
         <f>Public!A3</f>
-        <v>Thursday, February 06, 2020 02:35:47 PM</v>
+        <v>Monday, February 10, 2020 08:22:23 PM</v>
       </c>
       <c r="C3" s="14" t="str">
         <f>Public!B3</f>
-        <v>Keith Hang</v>
+        <v>吳天豐</v>
       </c>
       <c r="D3" s="14" t="str">
         <f>Public!C3</f>
-        <v>口罩漂白水酒精
-溝死女
-駛Q買你d珠仔💪🏻</v>
+        <v>圖中二人有否先洗手？</v>
       </c>
       <c r="F3" s="14" t="str">
         <f>Public!D3</f>
-        <v>https://www.facebook.com/153753694819713/posts/1251808008347604/?comment_id=1253322551529483</v>
+        <v>https://www.facebook.com/PandoraHongKong/photos/a.156393951222354/1255043328024072/?type=3&amp;comment_id=1256555641206174</v>
       </c>
       <c r="G3" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1804,19 +1753,19 @@
       </c>
       <c r="B4" s="6" t="str">
         <f>Public!A4</f>
-        <v>Thursday, February 06, 2020 04:42:38 PM</v>
+        <v>Monday, February 10, 2020 08:36:42 PM</v>
       </c>
       <c r="C4" s="14" t="str">
         <f>Public!B4</f>
-        <v>Lok Daisy</v>
+        <v>Tszyeung Li</v>
       </c>
       <c r="D4" s="14" t="str">
         <f>Public!C4</f>
-        <v>拎條鍊去洗，會屈你條鍊用洗銀水浸過，然後同你講洗唔到原來既色架！仲買？</v>
+        <v>港女鏈</v>
       </c>
       <c r="F4" s="14" t="str">
         <f>Public!D4</f>
-        <v>https://www.facebook.com/153753694819713/posts/2240275839408885/?comment_id=2240277299408739</v>
+        <v>https://www.facebook.com/PandoraHongKong/photos/a.156393951222354/1255043328024072/?type=3&amp;comment_id=1256563117872093</v>
       </c>
       <c r="G4" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1829,50 +1778,47 @@
       </c>
       <c r="B5" s="6" t="str">
         <f>Public!A5</f>
-        <v>Thursday, February 06, 2020 06:58:27 PM</v>
+        <v>Monday, February 10, 2020 10:53:00 PM</v>
       </c>
       <c r="C5" s="14" t="str">
         <f>Public!B5</f>
-        <v>Beau Manuswee</v>
+        <v>Jason Wong</v>
       </c>
       <c r="D5" s="14" t="str">
         <f>Public!C5</f>
-        <v>Gift Kumpunthong อิอิ เพื่อคันๆๆๆ</v>
-      </c>
-      <c r="E5" s="14" t="s">
-        <v>61</v>
+        <v>咁多首飾品牌，我最佩服Pandora，公園石春都賣到錢。。。。</v>
       </c>
       <c r="F5" s="14" t="str">
         <f>Public!D5</f>
-        <v>https://www.facebook.com/153753694819713/posts/1249085878619817/?comment_id=1253444781517260</v>
+        <v>https://www.facebook.com/PandoraHongKong/photos/a.156393951222354/1255043328024072/?type=3&amp;comment_id=1256644537863951</v>
       </c>
       <c r="G5" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>Other</v>
+        <v/>
       </c>
     </row>
     <row r="6" s="14" customFormat="1" spans="1:7">
       <c r="A6" s="14">
         <v>5</v>
       </c>
-      <c r="B6" s="6" t="str">
+      <c r="B6" s="6">
         <f>Public!A6</f>
-        <v>Thursday, February 06, 2020 11:28:10 PM</v>
-      </c>
-      <c r="C6" s="14" t="str">
+        <v>0</v>
+      </c>
+      <c r="C6" s="14">
         <f>Public!B6</f>
-        <v>May Yuen</v>
-      </c>
-      <c r="D6" s="14" t="str">
+        <v>0</v>
+      </c>
+      <c r="D6" s="14">
         <f>Public!C6</f>
-        <v>請問米奇要幾錢</v>
+        <v>0</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="F6" s="14" t="str">
+        <v>57</v>
+      </c>
+      <c r="F6" s="14">
         <f>Public!D6</f>
-        <v>https://www.facebook.com/153753694819713/posts/1242183959310009/?comment_id=1253608004834271</v>
+        <v>0</v>
       </c>
       <c r="G6" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1883,21 +1829,21 @@
       <c r="A7" s="14">
         <v>6</v>
       </c>
-      <c r="B7" s="6" t="str">
+      <c r="B7" s="6">
         <f>Public!A7</f>
-        <v>Friday, February 07, 2020 08:31:24 AM</v>
-      </c>
-      <c r="C7" s="14" t="str">
+        <v>0</v>
+      </c>
+      <c r="C7" s="14">
         <f>Public!B7</f>
-        <v>Mavis Law</v>
-      </c>
-      <c r="D7" s="14" t="str">
+        <v>0</v>
+      </c>
+      <c r="D7" s="14">
         <f>Public!C7</f>
-        <v>Koey Wai Cherry Yeung</v>
-      </c>
-      <c r="F7" s="14" t="str">
+        <v>0</v>
+      </c>
+      <c r="F7" s="14">
         <f>Public!D7</f>
-        <v>https://www.facebook.com/153753694819713/posts/1251251691736569/?comment_id=1253890828139322</v>
+        <v>0</v>
       </c>
       <c r="G7" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1908,24 +1854,24 @@
       <c r="A8" s="14">
         <v>7</v>
       </c>
-      <c r="B8" s="6" t="str">
+      <c r="B8" s="6">
         <f>Public!A8</f>
-        <v>Friday, February 07, 2020 12:03:19 PM</v>
-      </c>
-      <c r="C8" s="14" t="str">
+        <v>0</v>
+      </c>
+      <c r="C8" s="14">
         <f>Public!B8</f>
-        <v>Fanny Tam</v>
-      </c>
-      <c r="D8" s="14" t="str">
+        <v>0</v>
+      </c>
+      <c r="D8" s="14">
         <f>Public!C8</f>
-        <v>買滿幾錢？</v>
+        <v>0</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="F8" s="14" t="str">
+        <v>57</v>
+      </c>
+      <c r="F8" s="14">
         <f>Public!D8</f>
-        <v>https://www.facebook.com/153753694819713/posts/1251251691736569/?comment_id=1253995441462194</v>
+        <v>0</v>
       </c>
       <c r="G8" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1936,21 +1882,21 @@
       <c r="A9" s="14">
         <v>8</v>
       </c>
-      <c r="B9" s="6" t="str">
+      <c r="B9" s="6">
         <f>Public!A9</f>
-        <v>Friday, February 07, 2020 01:49:29 PM</v>
-      </c>
-      <c r="C9" s="14" t="str">
+        <v>0</v>
+      </c>
+      <c r="C9" s="14">
         <f>Public!B9</f>
-        <v>Keong Keong</v>
-      </c>
-      <c r="D9" s="14" t="str">
+        <v>0</v>
+      </c>
+      <c r="D9" s="14">
         <f>Public!C9</f>
-        <v>就像愛情，找帥哥破處X膜，然後被拋棄，留下永久撕裂傷，開始放盪，在去做處X膜手術，然後找好騙工具人，一帥哥渣男多處X制，聽歌聽到腦殘，該感動不感動，亂享受感動，越漂亮曾墮胎機率越高👺👺👺👹👹👹</v>
-      </c>
-      <c r="F9" s="14" t="str">
+        <v>0</v>
+      </c>
+      <c r="F9" s="14">
         <f>Public!D9</f>
-        <v>https://www.facebook.com/PandoraHongKong/photos/a.156393951222354/1251221261739612/?type=3&amp;comment_id=1254066051455133</v>
+        <v>0</v>
       </c>
       <c r="G9" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1961,21 +1907,21 @@
       <c r="A10" s="14">
         <v>9</v>
       </c>
-      <c r="B10" s="6" t="str">
+      <c r="B10" s="6">
         <f>Public!A10</f>
-        <v>Friday, February 07, 2020 02:23:06 PM</v>
-      </c>
-      <c r="C10" s="14" t="str">
+        <v>0</v>
+      </c>
+      <c r="C10" s="14">
         <f>Public!B10</f>
-        <v>Cherry Yeung</v>
-      </c>
-      <c r="D10" s="14" t="str">
+        <v>0</v>
+      </c>
+      <c r="D10" s="14">
         <f>Public!C10</f>
-        <v>Mavis Law 咁要集結去睇喎🤣</v>
-      </c>
-      <c r="F10" s="14" t="str">
+        <v>0</v>
+      </c>
+      <c r="F10" s="14">
         <f>Public!D10</f>
-        <v>https://www.facebook.com/153753694819713/posts/1251251691736569/?comment_id=1253890828139322&amp;reply_comment_id=1254083041453434</v>
+        <v>0</v>
       </c>
       <c r="G10" s="3" t="str">
         <f t="shared" si="0"/>
@@ -7844,7 +7790,7 @@
   <dimension ref="A1:G572"/>
   <sheetViews>
     <sheetView showZeros="0" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14" outlineLevelCol="6"/>
@@ -7858,25 +7804,25 @@
   <sheetData>
     <row r="1" s="14" customFormat="1" spans="1:7">
       <c r="A1" s="14" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D1" s="14" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F1" s="14" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" s="14" customFormat="1" spans="1:7">
@@ -7885,15 +7831,15 @@
       </c>
       <c r="B2" s="6" t="str">
         <f>Private!A2</f>
-        <v>Wednesday, January 08, 2020 12:08:11 PM</v>
+        <v>Monday, February 10, 2020 03:42:11 PM</v>
       </c>
       <c r="C2" s="14" t="str">
         <f>Private!B2</f>
-        <v>Anna Fung</v>
+        <v>Leung Wan Ko</v>
       </c>
       <c r="D2" s="14" t="str">
         <f>Private!C2</f>
-        <v>我肯定你post嘅時候大部份早已冇貨！咁係咪要問問海關商品說明條例呢？</v>
+        <v>https://s3.amazonaws.com/spr-uploads-prod/815/FACEBOOK/82906/media/871187EE4A4126C860B609668FFB1D47</v>
       </c>
       <c r="F2" s="14" t="str">
         <f>Private!D2</f>
@@ -7910,15 +7856,15 @@
       </c>
       <c r="B3" s="6" t="str">
         <f>Private!A3</f>
-        <v>Wednesday, January 08, 2020 03:49:10 PM</v>
+        <v>Monday, February 10, 2020 03:42:34 PM</v>
       </c>
       <c r="C3" s="14" t="str">
         <f>Private!B3</f>
-        <v>Bleu Loi</v>
+        <v>Leung Wan Ko</v>
       </c>
       <c r="D3" s="14" t="str">
         <f>Private!C3</f>
-        <v>我已經電郵了pap.cs@Pandora.net，但Katie沒有提供令人滿意的答覆，加上除此以外也沒有人回覆。她說我退回貨品後幾天可收回款項，但已經12天了，若然再沒有回覆，我會到警署和海關備案。</v>
+        <v>請問還有哩只款嗎？</v>
       </c>
       <c r="F3" s="14" t="str">
         <f>Private!D3</f>
@@ -7935,15 +7881,16 @@
       </c>
       <c r="B4" s="6" t="str">
         <f>Private!A4</f>
-        <v>Thursday, February 06, 2020 02:33:51 PM</v>
+        <v>Monday, February 10, 2020 05:25:54 PM</v>
       </c>
       <c r="C4" s="14" t="str">
         <f>Private!B4</f>
-        <v>Kathy Ching</v>
+        <v>Wan Pong Tang</v>
       </c>
       <c r="D4" s="14" t="str">
         <f>Private!C4</f>
-        <v>i wanted to ask if there's stock of harry potter series in kings cross shop.  i have purchased on Tuesday already, thx</v>
+        <v>昨日落了order，今日未見有mail confirm，可以幫我跟進嗎？
+order no. PNDHK00668968</v>
       </c>
       <c r="F4" s="14" t="str">
         <f>Private!D4</f>
@@ -7960,17 +7907,15 @@
       </c>
       <c r="B5" s="6" t="str">
         <f>Private!A5</f>
-        <v>Friday, February 07, 2020 01:16:07 PM</v>
+        <v>Monday, February 10, 2020 05:37:24 PM</v>
       </c>
       <c r="C5" s="14" t="str">
         <f>Private!B5</f>
-        <v>Typ Wong</v>
+        <v>Dave Henz</v>
       </c>
       <c r="D5" s="14" t="str">
         <f>Private!C5</f>
-        <v>https://ezone.ulifestyle.com.hk/article/2557002
-【口罩開賣】理的口罩 HKTVmall 開賣！＄65 三十個！【附直購連結】 - ezone.hk - 網絡生活…
-l.facebook.com</v>
+        <v>Hi</v>
       </c>
       <c r="F5" s="14" t="str">
         <f>Private!D5</f>
@@ -7987,16 +7932,15 @@
       </c>
       <c r="B6" s="6" t="str">
         <f>Private!A6</f>
-        <v>Friday, February 07, 2020 02:42:50 PM</v>
+        <v>Monday, February 10, 2020 05:37:38 PM</v>
       </c>
       <c r="C6" s="14" t="str">
         <f>Private!B6</f>
-        <v>Lillian Li</v>
+        <v>Dave Henz</v>
       </c>
       <c r="D6" s="14" t="str">
         <f>Private!C6</f>
-        <v>我門市買夠數，有9折，已經試過起門市用到9折，但網上又話我電話沒有登記，請跟進！
-Tel: 62906286</v>
+        <v>I want to order this item</v>
       </c>
       <c r="F6" s="14" t="str">
         <f>Private!D6</f>
@@ -8013,15 +7957,15 @@
       </c>
       <c r="B7" s="6" t="str">
         <f>Private!A7</f>
-        <v>Friday, February 07, 2020 02:43:06 PM</v>
+        <v>Monday, February 10, 2020 05:37:43 PM</v>
       </c>
       <c r="C7" s="14" t="str">
         <f>Private!B7</f>
-        <v>Lillian Li</v>
+        <v>Dave Henz</v>
       </c>
       <c r="D7" s="14" t="str">
         <f>Private!C7</f>
-        <v>https://s3.amazonaws.com/spr-uploads-prod/815/FACEBOOK/82906/media/F288E0AB9EF90AFF734CCA123FC44B2A</v>
+        <v>do you have</v>
       </c>
       <c r="F7" s="14" t="str">
         <f>Private!D7</f>
@@ -8036,21 +7980,21 @@
       <c r="A8" s="14">
         <v>7</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="6" t="str">
         <f>Private!A8</f>
-        <v>0</v>
-      </c>
-      <c r="C8" s="14">
+        <v>Monday, February 10, 2020 05:37:48 PM</v>
+      </c>
+      <c r="C8" s="14" t="str">
         <f>Private!B8</f>
-        <v>0</v>
-      </c>
-      <c r="D8" s="14">
+        <v>Dave Henz</v>
+      </c>
+      <c r="D8" s="14" t="str">
         <f>Private!C8</f>
-        <v>0</v>
-      </c>
-      <c r="F8" s="14">
+        <v>https://s3.amazonaws.com/spr-uploads-prod/815/FACEBOOK/82906/media/F279C2ECD2CC380F0E54A0B4103F302C</v>
+      </c>
+      <c r="F8" s="14" t="str">
         <f>Private!D8</f>
-        <v>0</v>
+        <v>Inbox</v>
       </c>
       <c r="G8" s="3" t="str">
         <f t="shared" si="0"/>
@@ -8061,21 +8005,21 @@
       <c r="A9" s="14">
         <v>8</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="6" t="str">
         <f>Private!A9</f>
-        <v>0</v>
-      </c>
-      <c r="C9" s="14">
+        <v>Monday, February 10, 2020 06:28:45 PM</v>
+      </c>
+      <c r="C9" s="14" t="str">
         <f>Private!B9</f>
-        <v>0</v>
-      </c>
-      <c r="D9" s="14">
+        <v>Tim Wong</v>
+      </c>
+      <c r="D9" s="14" t="str">
         <f>Private!C9</f>
-        <v>0</v>
-      </c>
-      <c r="F9" s="14">
+        <v>請問現在落單13號或之前能收到嗎</v>
+      </c>
+      <c r="F9" s="14" t="str">
         <f>Private!D9</f>
-        <v>0</v>
+        <v>Inbox</v>
       </c>
       <c r="G9" s="3" t="str">
         <f t="shared" si="0"/>
@@ -8086,21 +8030,21 @@
       <c r="A10" s="14">
         <v>9</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="6" t="str">
         <f>Private!A10</f>
-        <v>0</v>
-      </c>
-      <c r="C10" s="14">
+        <v>Monday, February 10, 2020 06:56:08 PM</v>
+      </c>
+      <c r="C10" s="14" t="str">
         <f>Private!B10</f>
-        <v>0</v>
-      </c>
-      <c r="D10" s="14">
+        <v>Asellus Wong</v>
+      </c>
+      <c r="D10" s="14" t="str">
         <f>Private!C10</f>
-        <v>0</v>
-      </c>
-      <c r="F10" s="14">
+        <v>想問買滿$1380 送嘅頸鏈有幾長? 同埋個心心鏈嘴可唔可以拆落黎?</v>
+      </c>
+      <c r="F10" s="14" t="str">
         <f>Private!D10</f>
-        <v>0</v>
+        <v>Inbox</v>
       </c>
       <c r="G10" s="3" t="str">
         <f t="shared" si="0"/>
@@ -8111,21 +8055,21 @@
       <c r="A11" s="14">
         <v>10</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="6" t="str">
         <f>Private!A11</f>
-        <v>0</v>
-      </c>
-      <c r="C11" s="14">
+        <v>Monday, February 10, 2020 07:19:16 PM</v>
+      </c>
+      <c r="C11" s="14" t="str">
         <f>Private!B11</f>
-        <v>0</v>
-      </c>
-      <c r="D11" s="14">
+        <v>Wan Pong Tang</v>
+      </c>
+      <c r="D11" s="14" t="str">
         <f>Private!C11</f>
-        <v>0</v>
-      </c>
-      <c r="F11" s="14">
+        <v>順丰有資料了，thanks</v>
+      </c>
+      <c r="F11" s="14" t="str">
         <f>Private!D11</f>
-        <v>0</v>
+        <v>Inbox</v>
       </c>
       <c r="G11" s="3" t="str">
         <f t="shared" si="0"/>
@@ -8136,21 +8080,21 @@
       <c r="A12" s="14">
         <v>11</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="6" t="str">
         <f>Private!A12</f>
-        <v>0</v>
-      </c>
-      <c r="C12" s="14">
+        <v>Monday, February 10, 2020 11:29:52 PM</v>
+      </c>
+      <c r="C12" s="14" t="str">
         <f>Private!B12</f>
-        <v>0</v>
-      </c>
-      <c r="D12" s="14">
+        <v>Noona Rt</v>
+      </c>
+      <c r="D12" s="14" t="str">
         <f>Private!C12</f>
-        <v>0</v>
-      </c>
-      <c r="F12" s="14">
+        <v>你好，請問你地門巿有冇呢款耳環？</v>
+      </c>
+      <c r="F12" s="14" t="str">
         <f>Private!D12</f>
-        <v>0</v>
+        <v>Inbox</v>
       </c>
       <c r="G12" s="3" t="str">
         <f t="shared" si="0"/>
@@ -8161,21 +8105,21 @@
       <c r="A13" s="14">
         <v>12</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="6" t="str">
         <f>Private!A13</f>
-        <v>0</v>
-      </c>
-      <c r="C13" s="14">
+        <v>Monday, February 10, 2020 11:29:56 PM</v>
+      </c>
+      <c r="C13" s="14" t="str">
         <f>Private!B13</f>
-        <v>0</v>
-      </c>
-      <c r="D13" s="14">
+        <v>Noona Rt</v>
+      </c>
+      <c r="D13" s="14" t="str">
         <f>Private!C13</f>
-        <v>0</v>
-      </c>
-      <c r="F13" s="14">
+        <v>https://s3.amazonaws.com/spr-uploads-prod/815/FACEBOOK/82906/media/166DD8C359D7B67ECCE9B0BE8F585988</v>
+      </c>
+      <c r="F13" s="14" t="str">
         <f>Private!D13</f>
-        <v>0</v>
+        <v>Inbox</v>
       </c>
       <c r="G13" s="3" t="str">
         <f t="shared" si="0"/>
@@ -8186,21 +8130,21 @@
       <c r="A14" s="14">
         <v>13</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14" s="6" t="str">
         <f>Private!A14</f>
-        <v>0</v>
-      </c>
-      <c r="C14" s="14">
+        <v>Tuesday, February 11, 2020 10:52:57 AM</v>
+      </c>
+      <c r="C14" s="14" t="str">
         <f>Private!B14</f>
-        <v>0</v>
-      </c>
-      <c r="D14" s="14">
+        <v>Mabel Lam</v>
+      </c>
+      <c r="D14" s="14" t="str">
         <f>Private!C14</f>
-        <v>0</v>
-      </c>
-      <c r="F14" s="14">
+        <v>如果直接落門市有呢個款嗎？</v>
+      </c>
+      <c r="F14" s="14" t="str">
         <f>Private!D14</f>
-        <v>0</v>
+        <v>Inbox</v>
       </c>
       <c r="G14" s="3" t="str">
         <f t="shared" si="0"/>
@@ -13971,7 +13915,7 @@
     <sheetView showZeros="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
+      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14"/>
@@ -13991,34 +13935,34 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="28" customHeight="1" spans="1:10">
       <c r="A1" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" s="1" customFormat="1" spans="1:10">
@@ -14059,77 +14003,75 @@
         <v>No response required</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" s="1" customFormat="1" spans="1:9">
       <c r="A3" s="1">
         <f>raw_response!A3</f>
-        <v>63</v>
-      </c>
-      <c r="B3" s="1" t="str">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1">
         <f>raw_response!B3</f>
-        <v>Thursday, February 06, 2020 14:28:07</v>
-      </c>
-      <c r="C3" s="1" t="str">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1">
         <f>raw_response!C3</f>
-        <v>Helen Helen</v>
-      </c>
-      <c r="D3" s="1" t="str">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
         <f>raw_response!D3</f>
-        <v>我都覺得呢個牌子唔應該再買，因脱色好緊要。</v>
-      </c>
-      <c r="E3" s="8" t="str">
+        <v>0</v>
+      </c>
+      <c r="E3" s="8">
         <f t="shared" si="0"/>
-        <v>Hi Helen Helen，非常抱歉你有以上經歷。請你電郵至 pap.cs@Pandora.net 提供姓名、聯絡電話同詳情，我哋會作出跟進。多謝！</v>
-      </c>
-      <c r="F3" s="1" t="str">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1">
         <f>raw_response!F3</f>
-        <v>https://www.facebook.com/153753694819713/posts/1249085878619817/?comment_id=1253319778196427</v>
-      </c>
-      <c r="G3" s="8" t="str">
+        <v>0</v>
+      </c>
+      <c r="G3" s="8">
         <f>raw_response!G3</f>
-        <v>Complaints</v>
+        <v>0</v>
       </c>
       <c r="H3" s="10">
         <f>raw_response!H3</f>
         <v>0</v>
       </c>
-      <c r="I3" s="1" t="str">
+      <c r="I3" s="1">
         <f>raw_response!E3</f>
-        <v>Hi Helen Helen，非常抱歉你有以上經歷。請你電郵至 pap.cs@Pandora.net 提供姓名、聯絡電話同詳情，我哋會作出跟進。多謝！</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" s="1" customFormat="1" spans="1:9">
       <c r="A4" s="1">
         <f>raw_response!A4</f>
-        <v>64</v>
+        <v>0</v>
       </c>
       <c r="B4" s="1" t="str">
         <f>raw_response!B4</f>
-        <v>Thursday, February 06, 2020 14:35:47</v>
+        <v>Monday, February 10, 2020 17:37:48</v>
       </c>
       <c r="C4" s="1" t="str">
         <f>raw_response!C4</f>
-        <v>Keith Hang</v>
+        <v>Dave Henz</v>
       </c>
       <c r="D4" s="1" t="str">
         <f>raw_response!D4</f>
-        <v>口罩漂白水酒精
-溝死女
-駛Q買你d珠仔💪🏻</v>
+        <v>https://s3.amazonaws.com/spr-uploads-prod/815/FACEBOOK/82906/media/F279C2ECD2CC380F0E54A0B4103F302C</v>
       </c>
       <c r="E4" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>No response required</v>
+        <v>te</v>
       </c>
       <c r="F4" s="1" t="str">
         <f>raw_response!F4</f>
-        <v>https://www.facebook.com/153753694819713/posts/1251808008347604/?comment_id=1253322551529483</v>
+        <v>Inbox</v>
       </c>
       <c r="G4" s="8" t="str">
         <f>raw_response!G4</f>
-        <v>Other</v>
+        <v>General</v>
       </c>
       <c r="H4" s="10">
         <f>raw_response!H4</f>
@@ -14137,75 +14079,75 @@
       </c>
       <c r="I4" s="1" t="str">
         <f>raw_response!E4</f>
-        <v>No response required</v>
+        <v>te</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" spans="1:9">
       <c r="A5" s="1">
         <f>raw_response!A5</f>
-        <v>65</v>
-      </c>
-      <c r="B5" s="1" t="str">
+        <v>0</v>
+      </c>
+      <c r="B5" s="1">
         <f>raw_response!B5</f>
-        <v>Thursday, February 06, 2020 16:42:38</v>
-      </c>
-      <c r="C5" s="1" t="str">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1">
         <f>raw_response!C5</f>
-        <v>Lok Daisy</v>
-      </c>
-      <c r="D5" s="1" t="str">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1">
         <f>raw_response!D5</f>
-        <v>拎條鍊去洗，會屈你條鍊用洗銀水浸過，然後同你講洗唔到原來既色架！仲買？</v>
-      </c>
-      <c r="E5" s="8" t="str">
+        <v>0</v>
+      </c>
+      <c r="E5" s="8">
         <f t="shared" si="0"/>
-        <v>No response required</v>
-      </c>
-      <c r="F5" s="1" t="str">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1">
         <f>raw_response!F5</f>
-        <v>https://www.facebook.com/153753694819713/posts/2240275839408885/?comment_id=2240277299408739</v>
-      </c>
-      <c r="G5" s="8" t="str">
+        <v>0</v>
+      </c>
+      <c r="G5" s="8">
         <f>raw_response!G5</f>
-        <v>Complaints</v>
+        <v>0</v>
       </c>
       <c r="H5" s="10">
         <f>raw_response!H5</f>
         <v>0</v>
       </c>
-      <c r="I5" s="1" t="str">
+      <c r="I5" s="1">
         <f>raw_response!E5</f>
-        <v>No response required</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" spans="1:9">
       <c r="A6" s="1">
         <f>raw_response!A6</f>
-        <v>66</v>
+        <v>0</v>
       </c>
       <c r="B6" s="1" t="str">
         <f>raw_response!B6</f>
-        <v>Thursday, February 06, 2020 18:58:27</v>
+        <v>Monday, February 10, 2020 23:29:52</v>
       </c>
       <c r="C6" s="1" t="str">
         <f>raw_response!C6</f>
-        <v>Beau Manuswee</v>
+        <v>Noona Rt</v>
       </c>
       <c r="D6" s="1" t="str">
         <f>raw_response!D6</f>
-        <v>Gift Kumpunthong อิอิ เพื่อคันๆๆๆ</v>
+        <v>你好，請問你地門巿有冇呢款耳環？</v>
       </c>
       <c r="E6" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>No response required</v>
+        <v>ttt</v>
       </c>
       <c r="F6" s="1" t="str">
         <f>raw_response!F6</f>
-        <v>https://www.facebook.com/153753694819713/posts/1249085878619817/?comment_id=1253444781517260</v>
+        <v>Inbox</v>
       </c>
       <c r="G6" s="8" t="str">
         <f>raw_response!G6</f>
-        <v>Other</v>
+        <v>General</v>
       </c>
       <c r="H6" s="10">
         <f>raw_response!H6</f>
@@ -14213,393 +14155,387 @@
       </c>
       <c r="I6" s="1" t="str">
         <f>raw_response!E6</f>
-        <v>No response required</v>
+        <v>ttt</v>
       </c>
     </row>
     <row r="7" s="1" customFormat="1" spans="1:9">
       <c r="A7" s="1">
         <f>raw_response!A7</f>
-        <v>67</v>
-      </c>
-      <c r="B7" s="1" t="str">
+        <v>0</v>
+      </c>
+      <c r="B7" s="1">
         <f>raw_response!B7</f>
-        <v>Thursday, February 06, 2020 21:43:47</v>
-      </c>
-      <c r="C7" s="1" t="str">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1">
         <f>raw_response!C7</f>
-        <v>Lok Daisy</v>
-      </c>
-      <c r="D7" s="1" t="str">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1">
         <f>raw_response!D7</f>
-        <v>拎條鍊去洗，會屈你條鍊用洗銀水浸過，然後同你講洗唔到原來既色架！仲買？</v>
-      </c>
-      <c r="E7" s="8" t="str">
+        <v>0</v>
+      </c>
+      <c r="E7" s="8">
         <f t="shared" si="0"/>
-        <v>No response required</v>
-      </c>
-      <c r="F7" s="1" t="str">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1">
         <f>raw_response!F7</f>
-        <v>https://www.facebook.com/153753694819713/posts/2790696994324388/?comment_id=2790697870990967</v>
-      </c>
-      <c r="G7" s="8" t="str">
+        <v>0</v>
+      </c>
+      <c r="G7" s="8">
         <f>raw_response!G7</f>
-        <v>Complaints</v>
+        <v>0</v>
       </c>
       <c r="H7" s="10">
         <f>raw_response!H7</f>
         <v>0</v>
       </c>
-      <c r="I7" s="1" t="str">
+      <c r="I7" s="1">
         <f>raw_response!E7</f>
-        <v>No response required</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" s="1" customFormat="1" spans="1:9">
       <c r="A8" s="1">
         <f>raw_response!A8</f>
-        <v>68</v>
-      </c>
-      <c r="B8" s="1" t="str">
+        <v>0</v>
+      </c>
+      <c r="B8" s="1">
         <f>raw_response!B8</f>
-        <v>Thursday, February 06, 2020 23:28:10</v>
-      </c>
-      <c r="C8" s="1" t="str">
+        <v>0</v>
+      </c>
+      <c r="C8" s="1">
         <f>raw_response!C8</f>
-        <v>May Yuen</v>
-      </c>
-      <c r="D8" s="1" t="str">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1">
         <f>raw_response!D8</f>
-        <v>請問米奇要幾錢</v>
-      </c>
-      <c r="E8" s="8" t="str">
+        <v>0</v>
+      </c>
+      <c r="E8" s="8">
         <f t="shared" si="0"/>
-        <v>Hi May Yuen，請到 https://go.pandora.net/2SqrqAj 查閱價錢，多謝你嘅支持！</v>
-      </c>
-      <c r="F8" s="1" t="str">
+        <v>0</v>
+      </c>
+      <c r="F8" s="1">
         <f>raw_response!F8</f>
-        <v>https://www.facebook.com/153753694819713/posts/1242183959310009/?comment_id=1253608004834271</v>
-      </c>
-      <c r="G8" s="8" t="str">
+        <v>0</v>
+      </c>
+      <c r="G8" s="8">
         <f>raw_response!G8</f>
-        <v>General</v>
+        <v>0</v>
       </c>
       <c r="H8" s="10">
         <f>raw_response!H8</f>
         <v>0</v>
       </c>
-      <c r="I8" s="1" t="str">
+      <c r="I8" s="1">
         <f>raw_response!E8</f>
-        <v>Hi May Yuen，請到 https://go.pandora.net/2SqrqAj 查閱價錢，多謝你嘅支持！</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" s="1" customFormat="1" spans="1:9">
       <c r="A9" s="1">
         <f>raw_response!A9</f>
-        <v>69</v>
-      </c>
-      <c r="B9" s="1" t="str">
+        <v>0</v>
+      </c>
+      <c r="B9" s="1">
         <f>raw_response!B9</f>
-        <v>Friday, February 07, 2020 08:31:24</v>
-      </c>
-      <c r="C9" s="1" t="str">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1">
         <f>raw_response!C9</f>
-        <v>Mavis Law</v>
-      </c>
-      <c r="D9" s="1" t="str">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1">
         <f>raw_response!D9</f>
-        <v>Koey Wai Cherry Yeung</v>
-      </c>
-      <c r="E9" s="8" t="str">
+        <v>0</v>
+      </c>
+      <c r="E9" s="8">
         <f t="shared" si="0"/>
-        <v>No response required</v>
-      </c>
-      <c r="F9" s="1" t="str">
+        <v>0</v>
+      </c>
+      <c r="F9" s="1">
         <f>raw_response!F9</f>
-        <v>https://www.facebook.com/153753694819713/posts/1251251691736569/?comment_id=1253890828139322</v>
-      </c>
-      <c r="G9" s="8" t="str">
+        <v>0</v>
+      </c>
+      <c r="G9" s="8">
         <f>raw_response!G9</f>
-        <v>Other</v>
+        <v>0</v>
       </c>
       <c r="H9" s="10">
         <f>raw_response!H9</f>
         <v>0</v>
       </c>
-      <c r="I9" s="1" t="str">
+      <c r="I9" s="1">
         <f>raw_response!E9</f>
-        <v>No response required</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" s="1" customFormat="1" spans="1:9">
       <c r="A10" s="1">
         <f>raw_response!A10</f>
-        <v>70</v>
-      </c>
-      <c r="B10" s="1" t="str">
+        <v>0</v>
+      </c>
+      <c r="B10" s="1">
         <f>raw_response!B10</f>
-        <v>Thursday, February 06, 2020 14:33:51</v>
-      </c>
-      <c r="C10" s="1" t="str">
+        <v>0</v>
+      </c>
+      <c r="C10" s="1">
         <f>raw_response!C10</f>
-        <v>Kathy Ching</v>
-      </c>
-      <c r="D10" s="1" t="str">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1">
         <f>raw_response!D10</f>
-        <v>i wanted to ask if there's stock of harry potter series in kings cross shop.  i have purchased on Tuesday already, thx</v>
-      </c>
-      <c r="E10" s="8" t="str">
+        <v>0</v>
+      </c>
+      <c r="E10" s="8">
         <f t="shared" si="0"/>
-        <v>Hi Kathy Ching, thanks for supporting us! Love Pandora!</v>
-      </c>
-      <c r="F10" s="1" t="str">
+        <v>0</v>
+      </c>
+      <c r="F10" s="1">
         <f>raw_response!F10</f>
-        <v>Inbox</v>
-      </c>
-      <c r="G10" s="8" t="str">
+        <v>0</v>
+      </c>
+      <c r="G10" s="8">
         <f>raw_response!G10</f>
-        <v>Other</v>
+        <v>0</v>
       </c>
       <c r="H10" s="10">
         <f>raw_response!H10</f>
         <v>0</v>
       </c>
-      <c r="I10" s="1" t="str">
+      <c r="I10" s="1">
         <f>raw_response!E10</f>
-        <v>Hi Kathy Ching, thanks for supporting us! Love Pandora!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" s="1" customFormat="1" spans="1:9">
       <c r="A11" s="1">
         <f>raw_response!A11</f>
-        <v>71</v>
-      </c>
-      <c r="B11" s="1" t="str">
+        <v>0</v>
+      </c>
+      <c r="B11" s="1">
         <f>raw_response!B11</f>
-        <v>Friday, February 07, 2020 12:03:19</v>
-      </c>
-      <c r="C11" s="1" t="str">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1">
         <f>raw_response!C11</f>
-        <v>Fanny Tam</v>
-      </c>
-      <c r="D11" s="1" t="str">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1">
         <f>raw_response!D11</f>
-        <v>買滿幾錢？</v>
-      </c>
-      <c r="E11" s="8" t="str">
+        <v>0</v>
+      </c>
+      <c r="E11" s="8">
         <f t="shared" si="0"/>
-        <v>Hi Fanny Tam，而家喺網店同專門店消費淨值滿港幣$1,380，即可獲贈指定項鏈；
-淨值滿港幣$2,280，即可獲贈指定項鏈及耳環。優惠去到2020年2月15日 00:00，贈品數量有限，送完即止。多謝支持Pandora！</v>
-      </c>
-      <c r="F11" s="1" t="str">
+        <v>0</v>
+      </c>
+      <c r="F11" s="1">
         <f>raw_response!F11</f>
-        <v>https://www.facebook.com/153753694819713/posts/1251251691736569/?comment_id=1253995441462194</v>
-      </c>
-      <c r="G11" s="8" t="str">
+        <v>0</v>
+      </c>
+      <c r="G11" s="8">
         <f>raw_response!G11</f>
-        <v>General</v>
+        <v>0</v>
       </c>
       <c r="H11" s="10">
         <f>raw_response!H11</f>
         <v>0</v>
       </c>
-      <c r="I11" s="1" t="str">
+      <c r="I11" s="1">
         <f>raw_response!E11</f>
-        <v>Hi Fanny Tam，而家喺網店同專門店消費淨值滿港幣$1,380，即可獲贈指定項鏈；
-淨值滿港幣$2,280，即可獲贈指定項鏈及耳環。優惠去到2020年2月15日 00:00，贈品數量有限，送完即止。多謝支持Pandora！</v>
-      </c>
-    </row>
-    <row r="12" s="1" customFormat="1" spans="1:10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" s="1" customFormat="1" spans="1:9">
       <c r="A12" s="1">
         <f>raw_response!A12</f>
-        <v>72</v>
-      </c>
-      <c r="B12" s="1" t="str">
+        <v>0</v>
+      </c>
+      <c r="B12" s="1">
         <f>raw_response!B12</f>
-        <v>Friday, February 07, 2020 13:49:29</v>
-      </c>
-      <c r="C12" s="1" t="str">
+        <v>0</v>
+      </c>
+      <c r="C12" s="1">
         <f>raw_response!C12</f>
-        <v>Keong Keong</v>
-      </c>
-      <c r="D12" s="1" t="str">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1">
         <f>raw_response!D12</f>
-        <v>就像愛情，找帥哥破處X膜，然後被拋棄，留下永久撕裂傷，開始放盪，在去做處X膜手術，然後找好騙工具人，一帥哥渣男多處X制，聽歌聽到腦殘，該感動不感動，亂享受感動，越漂亮曾墮胎機率越高👺👺👺👹👹👹</v>
-      </c>
-      <c r="E12" s="8" t="str">
+        <v>0</v>
+      </c>
+      <c r="E12" s="8">
         <f t="shared" si="0"/>
-        <v>Hide this comment, mark as spam</v>
-      </c>
-      <c r="F12" s="1" t="str">
+        <v>0</v>
+      </c>
+      <c r="F12" s="1">
         <f>raw_response!F12</f>
-        <v>https://www.facebook.com/PandoraHongKong/photos/a.156393951222354/1251221261739612/?type=3&amp;comment_id=1254066051455133</v>
-      </c>
-      <c r="G12" s="8" t="str">
+        <v>0</v>
+      </c>
+      <c r="G12" s="8">
         <f>raw_response!G12</f>
-        <v>Other</v>
+        <v>0</v>
       </c>
       <c r="H12" s="10">
         <f>raw_response!H12</f>
         <v>0</v>
       </c>
-      <c r="I12" s="1" t="str">
+      <c r="I12" s="1">
         <f>raw_response!E12</f>
-        <v>Hide this comment, mark as spam</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>70</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" s="1" customFormat="1" spans="1:9">
       <c r="A13" s="1">
         <f>raw_response!A13</f>
-        <v>73</v>
-      </c>
-      <c r="B13" s="1" t="str">
+        <v>0</v>
+      </c>
+      <c r="B13" s="1">
         <f>raw_response!B13</f>
-        <v>Friday, February 07, 2020 14:23:06</v>
-      </c>
-      <c r="C13" s="1" t="str">
+        <v>0</v>
+      </c>
+      <c r="C13" s="1">
         <f>raw_response!C13</f>
-        <v>Cherry Yeung</v>
-      </c>
-      <c r="D13" s="1" t="str">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1">
         <f>raw_response!D13</f>
-        <v>Mavis Law 咁要集結去睇喎🤣</v>
-      </c>
-      <c r="E13" s="8" t="str">
+        <v>0</v>
+      </c>
+      <c r="E13" s="8">
         <f t="shared" si="0"/>
-        <v>No response required</v>
-      </c>
-      <c r="F13" s="1" t="str">
+        <v>0</v>
+      </c>
+      <c r="F13" s="1">
         <f>raw_response!F13</f>
-        <v>https://www.facebook.com/153753694819713/posts/1251251691736569/?comment_id=1253890828139322&amp;reply_comment_id=1254083041453434</v>
-      </c>
-      <c r="G13" s="8" t="str">
+        <v>0</v>
+      </c>
+      <c r="G13" s="8">
         <f>raw_response!G13</f>
-        <v>Other</v>
+        <v>0</v>
       </c>
       <c r="H13" s="10">
         <f>raw_response!H13</f>
         <v>0</v>
       </c>
-      <c r="I13" s="1" t="str">
+      <c r="I13" s="1">
         <f>raw_response!E13</f>
-        <v>No response required</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" spans="1:9">
       <c r="A14" s="1">
         <f>raw_response!A14</f>
-        <v>74</v>
-      </c>
-      <c r="B14" s="1" t="str">
+        <v>0</v>
+      </c>
+      <c r="B14" s="1">
         <f>raw_response!B14</f>
-        <v>Friday, February 07, 2020 13:16:07</v>
-      </c>
-      <c r="C14" s="1" t="str">
+        <v>0</v>
+      </c>
+      <c r="C14" s="1">
         <f>raw_response!C14</f>
-        <v>Typ Wong</v>
-      </c>
-      <c r="D14" s="1" t="str">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1">
         <f>raw_response!D14</f>
-        <v>https://ezone.ulifestyle.com.hk/article/2557002</v>
-      </c>
-      <c r="E14" s="8" t="str">
+        <v>0</v>
+      </c>
+      <c r="E14" s="8">
         <f t="shared" si="0"/>
-        <v>No response required</v>
-      </c>
-      <c r="F14" s="1" t="str">
+        <v>0</v>
+      </c>
+      <c r="F14" s="1">
         <f>raw_response!F14</f>
-        <v>Inbox</v>
-      </c>
-      <c r="G14" s="8" t="str">
+        <v>0</v>
+      </c>
+      <c r="G14" s="8">
         <f>raw_response!G14</f>
-        <v>Other</v>
+        <v>0</v>
       </c>
       <c r="H14" s="10">
         <f>raw_response!H14</f>
         <v>0</v>
       </c>
-      <c r="I14" s="1" t="str">
+      <c r="I14" s="1">
         <f>raw_response!E14</f>
-        <v>No response required</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" s="1" customFormat="1" spans="1:9">
       <c r="A15" s="1">
         <f>raw_response!A15</f>
-        <v>75</v>
-      </c>
-      <c r="B15" s="1" t="str">
+        <v>0</v>
+      </c>
+      <c r="B15" s="1">
         <f>raw_response!B15</f>
-        <v>Friday, February 07, 2020 14:42:50</v>
-      </c>
-      <c r="C15" s="1" t="str">
+        <v>0</v>
+      </c>
+      <c r="C15" s="1">
         <f>raw_response!C15</f>
-        <v>Lillian Li</v>
-      </c>
-      <c r="D15" s="1" t="str">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1">
         <f>raw_response!D15</f>
-        <v>我門市買夠數，有9折，已經試過起門市用到9折，但網上又話我電話沒有登記，請跟進！
-Tel: 62906286</v>
-      </c>
-      <c r="E15" s="8" t="str">
+        <v>0</v>
+      </c>
+      <c r="E15" s="8">
         <f t="shared" si="0"/>
-        <v>Hi Lillian Li，非常抱歉你有以上經歷。請你電郵至 pap.cs@Pandora.net 提供姓名、聯絡電話同詳情，我哋會作出跟進。多謝你嘅支持！</v>
-      </c>
-      <c r="F15" s="1" t="str">
+        <v>0</v>
+      </c>
+      <c r="F15" s="1">
         <f>raw_response!F15</f>
-        <v>Inbox</v>
-      </c>
-      <c r="G15" s="8" t="str">
+        <v>0</v>
+      </c>
+      <c r="G15" s="8">
         <f>raw_response!G15</f>
-        <v>General</v>
+        <v>0</v>
       </c>
       <c r="H15" s="10">
         <f>raw_response!H15</f>
         <v>0</v>
       </c>
-      <c r="I15" s="1" t="str">
+      <c r="I15" s="1">
         <f>raw_response!E15</f>
-        <v>Hi Lillian Li，非常抱歉你有以上經歷。請你電郵至 pap.cs@Pandora.net 提供姓名、聯絡電話同詳情，我哋會作出跟進。多謝你嘅支持！</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" s="1" customFormat="1" spans="1:9">
       <c r="A16" s="1">
         <f>raw_response!A16</f>
-        <v>76</v>
-      </c>
-      <c r="B16" s="1" t="str">
+        <v>0</v>
+      </c>
+      <c r="B16" s="1">
         <f>raw_response!B16</f>
-        <v>Friday, February 07, 2020 14:43:06</v>
-      </c>
-      <c r="C16" s="1" t="str">
+        <v>0</v>
+      </c>
+      <c r="C16" s="1">
         <f>raw_response!C16</f>
-        <v>Lillian Li</v>
-      </c>
-      <c r="D16" s="1" t="str">
+        <v>0</v>
+      </c>
+      <c r="D16" s="1">
         <f>raw_response!D16</f>
-        <v>https://s3.amazonaws.com/spr-uploads-prod/815/FACEBOOK/82906/media/F288E0AB9EF90AFF734CCA123FC44B2A</v>
-      </c>
-      <c r="E16" s="8" t="str">
+        <v>0</v>
+      </c>
+      <c r="E16" s="8">
         <f t="shared" si="0"/>
-        <v>No response required</v>
-      </c>
-      <c r="F16" s="1" t="str">
+        <v>0</v>
+      </c>
+      <c r="F16" s="1">
         <f>raw_response!F16</f>
-        <v>Inbox</v>
-      </c>
-      <c r="G16" s="8" t="str">
+        <v>0</v>
+      </c>
+      <c r="G16" s="8">
         <f>raw_response!G16</f>
-        <v>General</v>
+        <v>0</v>
       </c>
       <c r="H16" s="10">
         <f>raw_response!H16</f>
         <v>0</v>
       </c>
-      <c r="I16" s="1" t="str">
+      <c r="I16" s="1">
         <f>raw_response!E16</f>
-        <v>No response required</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" s="1" customFormat="1" spans="1:9">
@@ -15250,19 +15186,19 @@
     </row>
     <row r="34" s="1" customFormat="1" spans="1:9">
       <c r="A34" s="1">
-        <f>raw_response!A28</f>
+        <f>raw_response!A34</f>
         <v>0</v>
       </c>
       <c r="B34" s="1">
-        <f>raw_response!B28</f>
+        <f>raw_response!B34</f>
         <v>0</v>
       </c>
       <c r="C34" s="1">
-        <f>raw_response!C28</f>
+        <f>raw_response!C34</f>
         <v>0</v>
       </c>
       <c r="D34" s="1">
-        <f>raw_response!D28</f>
+        <f>raw_response!D34</f>
         <v>0</v>
       </c>
       <c r="E34" s="8">
@@ -15270,37 +15206,37 @@
         <v>0</v>
       </c>
       <c r="F34" s="1">
-        <f>raw_response!F28</f>
+        <f>raw_response!F34</f>
         <v>0</v>
       </c>
       <c r="G34" s="8">
-        <f>raw_response!G28</f>
+        <f>raw_response!G34</f>
         <v>0</v>
       </c>
       <c r="H34" s="10">
-        <f>raw_response!H28</f>
+        <f>raw_response!H34</f>
         <v>0</v>
       </c>
       <c r="I34" s="1">
-        <f>raw_response!E28</f>
+        <f>raw_response!E34</f>
         <v>0</v>
       </c>
     </row>
     <row r="35" s="1" customFormat="1" spans="1:9">
       <c r="A35" s="1">
-        <f>raw_response!A29</f>
+        <f>raw_response!A35</f>
         <v>0</v>
       </c>
       <c r="B35" s="1">
-        <f>raw_response!B29</f>
+        <f>raw_response!B35</f>
         <v>0</v>
       </c>
       <c r="C35" s="1">
-        <f>raw_response!C29</f>
+        <f>raw_response!C35</f>
         <v>0</v>
       </c>
       <c r="D35" s="1">
-        <f>raw_response!D29</f>
+        <f>raw_response!D35</f>
         <v>0</v>
       </c>
       <c r="E35" s="8">
@@ -15308,37 +15244,37 @@
         <v>0</v>
       </c>
       <c r="F35" s="1">
-        <f>raw_response!F29</f>
+        <f>raw_response!F35</f>
         <v>0</v>
       </c>
       <c r="G35" s="8">
-        <f>raw_response!G29</f>
+        <f>raw_response!G35</f>
         <v>0</v>
       </c>
       <c r="H35" s="10">
-        <f>raw_response!H29</f>
+        <f>raw_response!H35</f>
         <v>0</v>
       </c>
       <c r="I35" s="1">
-        <f>raw_response!E29</f>
+        <f>raw_response!E35</f>
         <v>0</v>
       </c>
     </row>
     <row r="36" s="1" customFormat="1" spans="1:9">
       <c r="A36" s="1">
-        <f>raw_response!A30</f>
+        <f>raw_response!A36</f>
         <v>0</v>
       </c>
       <c r="B36" s="1">
-        <f>raw_response!B30</f>
+        <f>raw_response!B36</f>
         <v>0</v>
       </c>
       <c r="C36" s="1">
-        <f>raw_response!C30</f>
+        <f>raw_response!C36</f>
         <v>0</v>
       </c>
       <c r="D36" s="1">
-        <f>raw_response!D30</f>
+        <f>raw_response!D36</f>
         <v>0</v>
       </c>
       <c r="E36" s="8">
@@ -15346,37 +15282,37 @@
         <v>0</v>
       </c>
       <c r="F36" s="1">
-        <f>raw_response!F30</f>
+        <f>raw_response!F36</f>
         <v>0</v>
       </c>
       <c r="G36" s="8">
-        <f>raw_response!G30</f>
+        <f>raw_response!G36</f>
         <v>0</v>
       </c>
       <c r="H36" s="10">
-        <f>raw_response!H30</f>
+        <f>raw_response!H36</f>
         <v>0</v>
       </c>
       <c r="I36" s="1">
-        <f>raw_response!E30</f>
+        <f>raw_response!E36</f>
         <v>0</v>
       </c>
     </row>
     <row r="37" s="1" customFormat="1" spans="1:9">
       <c r="A37" s="1">
-        <f>raw_response!A31</f>
+        <f>raw_response!A37</f>
         <v>0</v>
       </c>
       <c r="B37" s="1">
-        <f>raw_response!B31</f>
+        <f>raw_response!B37</f>
         <v>0</v>
       </c>
       <c r="C37" s="1">
-        <f>raw_response!C31</f>
+        <f>raw_response!C37</f>
         <v>0</v>
       </c>
       <c r="D37" s="1">
-        <f>raw_response!D31</f>
+        <f>raw_response!D37</f>
         <v>0</v>
       </c>
       <c r="E37" s="8">
@@ -15384,37 +15320,37 @@
         <v>0</v>
       </c>
       <c r="F37" s="1">
-        <f>raw_response!F31</f>
+        <f>raw_response!F37</f>
         <v>0</v>
       </c>
       <c r="G37" s="8">
-        <f>raw_response!G31</f>
+        <f>raw_response!G37</f>
         <v>0</v>
       </c>
       <c r="H37" s="10">
-        <f>raw_response!H31</f>
+        <f>raw_response!H37</f>
         <v>0</v>
       </c>
       <c r="I37" s="1">
-        <f>raw_response!E31</f>
+        <f>raw_response!E37</f>
         <v>0</v>
       </c>
     </row>
     <row r="38" s="1" customFormat="1" spans="1:9">
       <c r="A38" s="1">
-        <f>raw_response!A32</f>
+        <f>raw_response!A38</f>
         <v>0</v>
       </c>
       <c r="B38" s="1">
-        <f>raw_response!B32</f>
+        <f>raw_response!B38</f>
         <v>0</v>
       </c>
       <c r="C38" s="1">
-        <f>raw_response!C32</f>
+        <f>raw_response!C38</f>
         <v>0</v>
       </c>
       <c r="D38" s="1">
-        <f>raw_response!D32</f>
+        <f>raw_response!D38</f>
         <v>0</v>
       </c>
       <c r="E38" s="8">
@@ -15422,37 +15358,37 @@
         <v>0</v>
       </c>
       <c r="F38" s="1">
-        <f>raw_response!F32</f>
+        <f>raw_response!F38</f>
         <v>0</v>
       </c>
       <c r="G38" s="8">
-        <f>raw_response!G32</f>
+        <f>raw_response!G38</f>
         <v>0</v>
       </c>
       <c r="H38" s="10">
-        <f>raw_response!H32</f>
+        <f>raw_response!H38</f>
         <v>0</v>
       </c>
       <c r="I38" s="1">
-        <f>raw_response!E32</f>
+        <f>raw_response!E38</f>
         <v>0</v>
       </c>
     </row>
     <row r="39" s="1" customFormat="1" spans="1:9">
       <c r="A39" s="1">
-        <f>raw_response!A33</f>
+        <f>raw_response!A39</f>
         <v>0</v>
       </c>
       <c r="B39" s="1">
-        <f>raw_response!B33</f>
+        <f>raw_response!B39</f>
         <v>0</v>
       </c>
       <c r="C39" s="1">
-        <f>raw_response!C33</f>
+        <f>raw_response!C39</f>
         <v>0</v>
       </c>
       <c r="D39" s="1">
-        <f>raw_response!D33</f>
+        <f>raw_response!D39</f>
         <v>0</v>
       </c>
       <c r="E39" s="8">
@@ -15460,19 +15396,19 @@
         <v>0</v>
       </c>
       <c r="F39" s="1">
-        <f>raw_response!F33</f>
+        <f>raw_response!F39</f>
         <v>0</v>
       </c>
       <c r="G39" s="8">
-        <f>raw_response!G33</f>
+        <f>raw_response!G39</f>
         <v>0</v>
       </c>
       <c r="H39" s="10">
-        <f>raw_response!H33</f>
+        <f>raw_response!H39</f>
         <v>0</v>
       </c>
       <c r="I39" s="1">
-        <f>raw_response!E33</f>
+        <f>raw_response!E39</f>
         <v>0</v>
       </c>
     </row>
@@ -23839,15 +23775,15 @@
   <dimension ref="A1:H566"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14" outlineLevelCol="7"/>
   <cols>
     <col min="1" max="1" width="4.09090909090909" style="1" customWidth="1"/>
-    <col min="2" max="2" width="35.3636363636364" style="2" customWidth="1"/>
+    <col min="2" max="2" width="40" style="2" customWidth="1"/>
     <col min="3" max="3" width="13.4545454545455" style="1" customWidth="1"/>
     <col min="4" max="4" width="19.4545454545455" style="1" customWidth="1"/>
     <col min="5" max="5" width="28.7272727272727" style="1" customWidth="1"/>
@@ -23860,446 +23796,320 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:8">
       <c r="A1" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" s="1" customFormat="1" spans="2:8">
       <c r="B2" s="6"/>
       <c r="E2" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="4"/>
     </row>
-    <row r="3" s="1" customFormat="1" spans="1:8">
-      <c r="A3" s="1">
-        <v>63</v>
-      </c>
-      <c r="B3" s="6" t="s">
+    <row r="3" s="1" customFormat="1" spans="2:8">
+      <c r="B3" s="6"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="4"/>
+    </row>
+    <row r="4" s="1" customFormat="1" ht="42" customHeight="1" spans="2:8">
+      <c r="B4" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="H4" s="4"/>
+    </row>
+    <row r="5" s="1" customFormat="1" spans="2:8">
+      <c r="B5" s="6"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="4"/>
+    </row>
+    <row r="6" s="1" customFormat="1" spans="2:8">
+      <c r="B6" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="H3" s="4"/>
-    </row>
-    <row r="4" s="1" customFormat="1" ht="42" spans="1:8">
-      <c r="A4" s="1">
-        <v>64</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="H4" s="4"/>
-    </row>
-    <row r="5" s="1" customFormat="1" spans="1:8">
-      <c r="A5" s="1">
-        <v>65</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="H5" s="4"/>
-    </row>
-    <row r="6" s="1" customFormat="1" spans="1:8">
-      <c r="A6" s="1">
-        <v>66</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="F6" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="H6" s="4"/>
     </row>
-    <row r="7" s="1" customFormat="1" spans="1:8">
-      <c r="A7" s="1">
-        <v>67</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>74</v>
-      </c>
+    <row r="7" s="1" customFormat="1" spans="2:8">
+      <c r="B7" s="6"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="3"/>
       <c r="H7" s="4"/>
     </row>
-    <row r="8" s="1" customFormat="1" spans="1:8">
-      <c r="A8" s="1">
-        <v>68</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>83</v>
-      </c>
+    <row r="8" s="1" customFormat="1" spans="2:8">
+      <c r="B8" s="6"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="3"/>
       <c r="H8" s="4"/>
     </row>
-    <row r="9" s="1" customFormat="1" spans="1:8">
-      <c r="A9" s="1">
-        <v>69</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>76</v>
-      </c>
+    <row r="9" s="1" customFormat="1" spans="2:8">
+      <c r="B9" s="6"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="3"/>
       <c r="H9" s="4"/>
     </row>
-    <row r="10" s="1" customFormat="1" spans="1:8">
-      <c r="A10" s="1">
-        <v>70</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>76</v>
-      </c>
+    <row r="10" s="1" customFormat="1" spans="2:8">
+      <c r="B10" s="6"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="3"/>
       <c r="H10" s="4"/>
     </row>
-    <row r="11" s="1" customFormat="1" ht="112" spans="1:8">
-      <c r="A11" s="1">
-        <v>71</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>83</v>
-      </c>
+    <row r="11" s="1" customFormat="1" ht="112" customHeight="1" spans="2:8">
+      <c r="B11" s="6"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="3"/>
       <c r="H11" s="4"/>
     </row>
-    <row r="12" s="1" customFormat="1" spans="1:8">
-      <c r="A12" s="1">
-        <v>72</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>76</v>
-      </c>
+    <row r="12" s="1" customFormat="1" spans="2:8">
+      <c r="B12" s="6"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="3"/>
       <c r="H12" s="4"/>
     </row>
-    <row r="13" s="1" customFormat="1" spans="1:8">
-      <c r="A13" s="1">
-        <v>73</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>76</v>
-      </c>
+    <row r="13" s="1" customFormat="1" spans="2:8">
+      <c r="B13" s="6"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="3"/>
       <c r="H13" s="4"/>
     </row>
-    <row r="14" s="1" customFormat="1" spans="1:8">
-      <c r="A14" s="1">
-        <v>74</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>76</v>
-      </c>
+    <row r="14" s="1" customFormat="1" spans="2:8">
+      <c r="B14" s="6"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="3"/>
       <c r="H14" s="4"/>
     </row>
-    <row r="15" s="1" customFormat="1" ht="98" spans="1:8">
-      <c r="A15" s="1">
-        <v>75</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>83</v>
-      </c>
+    <row r="15" s="1" customFormat="1" ht="98" customHeight="1" spans="2:8">
+      <c r="B15" s="6"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="3"/>
       <c r="H15" s="4"/>
     </row>
-    <row r="16" s="1" customFormat="1" spans="1:8">
-      <c r="A16" s="1">
-        <v>76</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>83</v>
-      </c>
+    <row r="16" s="1" customFormat="1" spans="2:8">
+      <c r="B16" s="6"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="3"/>
       <c r="H16" s="4"/>
     </row>
     <row r="17" s="1" customFormat="1" spans="2:8">
       <c r="B17" s="6"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
       <c r="G17" s="3"/>
       <c r="H17" s="4"/>
     </row>
     <row r="18" s="1" customFormat="1" spans="2:8">
       <c r="B18" s="6"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
       <c r="G18" s="3"/>
       <c r="H18" s="4"/>
     </row>
     <row r="19" s="1" customFormat="1" spans="2:8">
       <c r="B19" s="6"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
       <c r="G19" s="3"/>
       <c r="H19" s="4"/>
     </row>
     <row r="20" s="1" customFormat="1" spans="2:8">
       <c r="B20" s="6"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
       <c r="G20" s="3"/>
       <c r="H20" s="4"/>
     </row>
     <row r="21" s="1" customFormat="1" spans="2:8">
       <c r="B21" s="6"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
       <c r="G21" s="3"/>
       <c r="H21" s="4"/>
     </row>
     <row r="22" s="1" customFormat="1" spans="2:8">
       <c r="B22" s="6"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
       <c r="G22" s="3"/>
       <c r="H22" s="4"/>
     </row>
     <row r="23" s="1" customFormat="1" spans="2:8">
       <c r="B23" s="6"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
       <c r="G23" s="3"/>
       <c r="H23" s="4"/>
     </row>
     <row r="24" s="1" customFormat="1" spans="2:8">
       <c r="B24" s="6"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
       <c r="G24" s="3"/>
       <c r="H24" s="4"/>
     </row>
     <row r="25" s="1" customFormat="1" spans="2:8">
       <c r="B25" s="6"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
       <c r="G25" s="3"/>
       <c r="H25" s="4"/>
     </row>
     <row r="26" s="1" customFormat="1" spans="2:8">
       <c r="B26" s="6"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
       <c r="G26" s="3"/>
       <c r="H26" s="4"/>
     </row>
     <row r="27" s="1" customFormat="1" spans="2:8">
       <c r="B27" s="6"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
       <c r="G27" s="3"/>
       <c r="H27" s="4"/>
     </row>
     <row r="28" s="1" customFormat="1" spans="2:8">
       <c r="B28" s="6"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
       <c r="G28" s="3"/>
       <c r="H28" s="4"/>
     </row>
-    <row r="29" s="1" customFormat="1" spans="2:8">
+    <row r="29" s="1" customFormat="1" ht="196" customHeight="1" spans="2:8">
       <c r="B29" s="6"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
       <c r="G29" s="3"/>
       <c r="H29" s="4"/>
     </row>
     <row r="30" s="1" customFormat="1" spans="2:8">
       <c r="B30" s="6"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
       <c r="G30" s="3"/>
       <c r="H30" s="4"/>
     </row>
-    <row r="31" s="1" customFormat="1" spans="2:8">
+    <row r="31" s="1" customFormat="1" ht="210" customHeight="1" spans="2:8">
       <c r="B31" s="6"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="1"/>
       <c r="G31" s="3"/>
       <c r="H31" s="4"/>
     </row>

</xml_diff>